<commit_message>
add lit results to mock community
</commit_message>
<xml_diff>
--- a/test-lane-1/results/EGC_mock_community_LerayXT.xlsx
+++ b/test-lane-1/results/EGC_mock_community_LerayXT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcf05\Documents\PhD\DNA_Metabarcoding\GreenCrab\EGC-Salish-Sea\test-lane-1\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AD43FB-D14D-47FF-847C-8FEC3FC0723D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFFF80B-4BA9-4DD1-BF1B-C7B17D0FF14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="130">
   <si>
     <t>Group</t>
   </si>
@@ -340,13 +340,111 @@
   </si>
   <si>
     <t>shrimp</t>
+  </si>
+  <si>
+    <t>additions from the literature</t>
+  </si>
+  <si>
+    <t>Mytilis spp</t>
+  </si>
+  <si>
+    <t>parameterized green crab bioenergetics model for Willapa Bay</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Present in Stevens et al. (1982)?</t>
+  </si>
+  <si>
+    <t>yes (Balanomorpha)</t>
+  </si>
+  <si>
+    <t>Macoma spp</t>
+  </si>
+  <si>
+    <t>Myidae</t>
+  </si>
+  <si>
+    <r>
+      <t>yes (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Crangon spp, franciscorum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Citharichthys sordidus</t>
+  </si>
+  <si>
+    <t>Ophiodon elongatus</t>
+  </si>
+  <si>
+    <t>Cryptomya sp.</t>
+  </si>
+  <si>
+    <t>Stevens et al. important in June</t>
+  </si>
+  <si>
+    <t>Stevens et al. important in Sept</t>
+  </si>
+  <si>
+    <t>Eogammarus spp</t>
+  </si>
+  <si>
+    <t>sanddab</t>
+  </si>
+  <si>
+    <t>lingcod</t>
+  </si>
+  <si>
+    <t>Ammodytes caItera</t>
+  </si>
+  <si>
+    <t>sand lance</t>
+  </si>
+  <si>
+    <t>soft-shell clam</t>
+  </si>
+  <si>
+    <t>clam</t>
+  </si>
+  <si>
+    <t>mussel</t>
+  </si>
+  <si>
+    <t>**Cordone et al. did pick up insect DNA (Chironomidae)</t>
+  </si>
+  <si>
+    <t>Blenniiformes</t>
+  </si>
+  <si>
+    <t>Cordone et al. identified with BF3/BR2 primer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,6 +581,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -837,7 +943,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -847,6 +953,8 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1202,19 +1310,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>81</v>
       </c>
@@ -1224,8 +1334,11 @@
       <c r="C1" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1236,7 +1349,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1247,7 +1360,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1258,7 +1371,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1269,7 +1382,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1280,7 +1393,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1290,8 +1403,11 @@
       <c r="C7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -1301,8 +1417,11 @@
       <c r="C8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1313,7 +1432,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -1324,7 +1443,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1335,7 +1454,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1346,7 +1465,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1357,7 +1476,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -1368,7 +1487,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1379,7 +1498,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -1390,7 +1509,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1401,12 +1520,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>102</v>
       </c>
@@ -1416,21 +1535,27 @@
       <c r="C20" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
@@ -1438,7 +1563,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>31</v>
       </c>
@@ -1446,7 +1571,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
@@ -1454,7 +1579,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>91</v>
       </c>
@@ -1462,8 +1587,99 @@
         <v>92</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>